<commit_message>
post commande & get commande finis
</commit_message>
<xml_diff>
--- a/conception/LBS-stories-LP1.xlsx
+++ b/conception/LBS-stories-LP1.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -181,7 +182,7 @@
     <t xml:space="preserve">obtenir la commande pour suivre son état</t>
   </si>
   <si>
-    <t xml:space="preserve">/commandes/{id}</t>
+    <t xml:space="preserve">/commandes/{id}?token={token}</t>
   </si>
   <si>
     <t xml:space="preserve">supprimer sandwich</t>
@@ -593,22 +594,22 @@
   <dimension ref="A1:V65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.7244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.2959183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.3010204081633"/>
-    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="18.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1292,9 +1293,11 @@
         <v>51</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -2111,7 +2114,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="11" t="n">
         <f aca="false">E7*H7+E8*H8+E9*H9+E10*H10+E11*H11+E12*H12+E13*H13+E14*H14+E15*H15+E16*H16+E17*H17+E18*H18+E19*H19+E20*H20+E21*H21+E22*H22</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>

</xml_diff>

<commit_message>
get carte + paiement carte
</commit_message>
<xml_diff>
--- a/conception/LBS-stories-LP1.xlsx
+++ b/conception/LBS-stories-LP1.xlsx
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -243,6 +244,9 @@
     <t xml:space="preserve">authentification  http basic, retourne un token jwt</t>
   </si>
   <si>
+    <t xml:space="preserve">/cartes/{id}/auth</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baptiste/Islam/Mohammed</t>
   </si>
   <si>
@@ -252,13 +256,16 @@
     <t xml:space="preserve">Accès à une carte : le token jwt est nécessaire</t>
   </si>
   <si>
-    <t xml:space="preserve">Mohammed</t>
+    <t xml:space="preserve">/cartes/{id}</t>
   </si>
   <si>
     <t xml:space="preserve">paiement fidélisé</t>
   </si>
   <si>
     <t xml:space="preserve">payer une commande en utilisant la carte : le montant est crédité sur la carte, on peut utiliser la réduction issue de la carte de fidélité – le montant cumulé est remis à 0 – le token jwt est nécessaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/cartes/{id}/paiement</t>
   </si>
   <si>
     <t xml:space="preserve">créer sa carte de fidélité</t>
@@ -606,22 +613,23 @@
   </sheetPr>
   <dimension ref="A1:V65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O28" activeCellId="0" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.3775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2755102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1528,7 +1536,9 @@
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="H25" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="I25" s="10"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1562,7 +1572,9 @@
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="H26" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="I26" s="10"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1596,7 +1608,9 @@
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="H27" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="I27" s="10"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1692,13 +1706,17 @@
       <c r="E30" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="10"/>
+      <c r="F30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="H30" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1722,21 +1740,25 @@
         <v>1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="10"/>
+      <c r="F31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="H31" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1760,18 +1782,26 @@
         <v>1</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E32" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
+      <c r="F32" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1794,10 +1824,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E33" s="11" t="n">
         <v>4</v>
@@ -1822,7 +1852,7 @@
     </row>
     <row r="34" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -1892,10 +1922,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E36" s="11" t="n">
         <v>3</v>
@@ -1926,10 +1956,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E37" s="11" t="n">
         <v>4</v>
@@ -1960,10 +1990,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E38" s="11" t="n">
         <v>4</v>
@@ -1994,10 +2024,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E39" s="11" t="n">
         <v>3</v>
@@ -2028,10 +2058,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E40" s="11" t="n">
         <v>4</v>
@@ -2062,10 +2092,10 @@
         <v>3</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E41" s="11" t="n">
         <v>4</v>
@@ -2141,8 +2171,8 @@
       <c r="C44" s="22"/>
       <c r="D44" s="12"/>
       <c r="E44" s="11" t="n">
-        <f aca="false">E7*H7+E8*H8+E9*H9+E10*H10+E11*H11+E12*H12+E13*H13+E14*H14+E15*H15+E16*H16+E17*H17+E18*H18+E19*H19+E20*H20+E21*H21+E22*H22</f>
-        <v>36</v>
+        <f aca="false">E7*H7+E8*H8+E9*H9+E10*H10+E11*H11+E12*H12+E13*H13+E14*H14+E15*H15+E16*H16+E17*H17+E18*H18+E19*H19+E20*H20+E21*H21+E22*H22+E25*H25+E26*H26+E27*H27+E30*H30+E31*H31+E32*H32+E33*H33+E36*H36+E37*H37+E38*H38+E39*H39+E40*H40+E41*H41</f>
+        <v>52</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2167,7 +2197,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="22"/>
       <c r="D45" s="23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E45" s="11" t="n">
         <f aca="false">SUM(E7:E22)+SUM(E25:E27)+SUM(E30:E33)+SUM(E36:E41)</f>

</xml_diff>

<commit_message>
paiement sand + docker gestion + gestion erreur auth
</commit_message>
<xml_diff>
--- a/conception/LBS-stories-LP1.xlsx
+++ b/conception/LBS-stories-LP1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">payer une commande en transmettant des coordonnées bancaires – (n°carte+date-expiration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/commandes/{id}/paiement?token={token}</t>
   </si>
   <si>
     <t xml:space="preserve">état de la commande</t>
@@ -613,8 +616,8 @@
   </sheetPr>
   <dimension ref="A1:V65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O28" activeCellId="0" sqref="O28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1279,11 +1282,15 @@
       <c r="F18" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1306,10 +1313,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E19" s="11" t="n">
         <v>2</v>
@@ -1318,7 +1325,7 @@
         <v>13</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H19" s="10" t="n">
         <v>1</v>
@@ -1348,16 +1355,16 @@
         <v>2</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E20" s="11" t="n">
         <v>3</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10" t="n">
@@ -1386,10 +1393,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" s="11" t="n">
         <v>3</v>
@@ -1424,10 +1431,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E22" s="11" t="n">
         <v>4</v>
@@ -1456,7 +1463,7 @@
     </row>
     <row r="23" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -1526,10 +1533,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E25" s="11" t="n">
         <v>3</v>
@@ -1562,10 +1569,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E26" s="11" t="n">
         <v>3</v>
@@ -1598,10 +1605,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E27" s="11" t="n">
         <v>3</v>
@@ -1628,7 +1635,7 @@
     </row>
     <row r="28" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -1698,10 +1705,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E30" s="11" t="n">
         <v>5</v>
@@ -1710,13 +1717,13 @@
         <v>13</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H30" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1740,10 +1747,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E31" s="11" t="n">
         <v>5</v>
@@ -1752,13 +1759,13 @@
         <v>13</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H31" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1782,10 +1789,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E32" s="11" t="n">
         <v>6</v>
@@ -1794,7 +1801,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H32" s="10" t="n">
         <v>1</v>
@@ -1824,10 +1831,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E33" s="11" t="n">
         <v>4</v>
@@ -1852,7 +1859,7 @@
     </row>
     <row r="34" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -1922,10 +1929,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E36" s="11" t="n">
         <v>3</v>
@@ -1956,10 +1963,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E37" s="11" t="n">
         <v>4</v>
@@ -1990,10 +1997,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E38" s="11" t="n">
         <v>4</v>
@@ -2024,10 +2031,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E39" s="11" t="n">
         <v>3</v>
@@ -2058,10 +2065,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E40" s="11" t="n">
         <v>4</v>
@@ -2092,10 +2099,10 @@
         <v>3</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E41" s="11" t="n">
         <v>4</v>
@@ -2172,7 +2179,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="11" t="n">
         <f aca="false">E7*H7+E8*H8+E9*H9+E10*H10+E11*H11+E12*H12+E13*H13+E14*H14+E15*H15+E16*H16+E17*H17+E18*H18+E19*H19+E20*H20+E21*H21+E22*H22+E25*H25+E26*H26+E27*H27+E30*H30+E31*H31+E32*H32+E33*H33+E36*H36+E37*H37+E38*H38+E39*H39+E40*H40+E41*H41</f>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2197,7 +2204,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="22"/>
       <c r="D45" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E45" s="11" t="n">
         <f aca="false">SUM(E7:E22)+SUM(E25:E27)+SUM(E30:E33)+SUM(E36:E41)</f>

</xml_diff>

<commit_message>
TWIG : theme, creer compte, liste categorie, liste sand par cat
</commit_message>
<xml_diff>
--- a/conception/LBS-stories-LP1.xlsx
+++ b/conception/LBS-stories-LP1.xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -112,7 +113,7 @@
     <t xml:space="preserve">obtenir la liste des sandwichs d'une catégorie</t>
   </si>
   <si>
-    <t xml:space="preserve">/categoires/{id}/sandwich</t>
+    <t xml:space="preserve">/categories/{id}/sandwich</t>
   </si>
   <si>
     <t xml:space="preserve">filtrage des sandwichs</t>
@@ -616,23 +617,23 @@
   </sheetPr>
   <dimension ref="A1:V65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1939,8 +1940,12 @@
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
+      <c r="H36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -2075,8 +2080,12 @@
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
+      <c r="H40" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -2179,7 +2188,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="11" t="n">
         <f aca="false">E7*H7+E8*H8+E9*H9+E10*H10+E11*H11+E12*H12+E13*H13+E14*H14+E15*H15+E16*H16+E17*H17+E18*H18+E19*H19+E20*H20+E21*H21+E22*H22+E25*H25+E26*H26+E27*H27+E30*H30+E31*H31+E32*H32+E33*H33+E36*H36+E37*H37+E38*H38+E39*H39+E40*H40+E41*H41</f>
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>

</xml_diff>

<commit_message>
deconnexion twig + fix
</commit_message>
<xml_diff>
--- a/conception/LBS-stories-LP1.xlsx
+++ b/conception/LBS-stories-LP1.xlsx
@@ -19,6 +19,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">Feuille1!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -176,7 +177,7 @@
     <t xml:space="preserve">/commandes/{id}</t>
   </si>
   <si>
-    <t xml:space="preserve">Daniel/Mohammed</t>
+    <t xml:space="preserve">Daniel/Mohammed/Baptiste/Islam</t>
   </si>
   <si>
     <t xml:space="preserve">Payer une commande</t>
@@ -227,6 +228,9 @@
     <t xml:space="preserve">liste des commandes, filtrées sur l'état , triée par date de livraison et ordre de création – permet au point de vente de planifier la préparation des commandes</t>
   </si>
   <si>
+    <t xml:space="preserve">Mohammed</t>
+  </si>
+  <si>
     <t xml:space="preserve">détail d'une commande</t>
   </si>
   <si>
@@ -239,6 +243,9 @@
     <t xml:space="preserve">changement de l'état d'une commande – vérification de la validité de la transition</t>
   </si>
   <si>
+    <t xml:space="preserve">/commandes/{id}/edit_state</t>
+  </si>
+  <si>
     <t xml:space="preserve">STORIES CONCERNANT LA GESTION DE LA CARTE DE FIDELITE</t>
   </si>
   <si>
@@ -287,6 +294,9 @@
     <t xml:space="preserve">lister les sandwichs  disponibles par catégories</t>
   </si>
   <si>
+    <t xml:space="preserve">/liste</t>
+  </si>
+  <si>
     <t xml:space="preserve">supprimer un sandwich</t>
   </si>
   <si>
@@ -309,6 +319,9 @@
   </si>
   <si>
     <t xml:space="preserve">identifiant + passwd – contrôle d'accès</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/connexion</t>
   </si>
   <si>
     <t xml:space="preserve">obtenir un TDB </t>
@@ -617,23 +630,23 @@
   </sheetPr>
   <dimension ref="A1:V65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="22" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1542,12 +1555,18 @@
       <c r="E25" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="10"/>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H25" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1570,20 +1589,26 @@
         <v>1</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E26" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10"/>
+      <c r="F26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="H26" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1606,20 +1631,26 @@
         <v>1</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E27" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="10"/>
+      <c r="F27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="H27" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1636,7 +1667,7 @@
     </row>
     <row r="28" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -1706,10 +1737,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E30" s="11" t="n">
         <v>5</v>
@@ -1718,13 +1749,13 @@
         <v>13</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H30" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1748,10 +1779,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E31" s="11" t="n">
         <v>5</v>
@@ -1760,13 +1791,13 @@
         <v>13</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H31" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1790,10 +1821,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E32" s="11" t="n">
         <v>6</v>
@@ -1802,7 +1833,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H32" s="10" t="n">
         <v>1</v>
@@ -1832,10 +1863,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E33" s="11" t="n">
         <v>4</v>
@@ -1860,7 +1891,7 @@
     </row>
     <row r="34" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -1930,16 +1961,20 @@
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E36" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="10"/>
+      <c r="F36" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="H36" s="10" t="n">
         <v>1</v>
       </c>
@@ -1968,10 +2003,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E37" s="11" t="n">
         <v>4</v>
@@ -2002,10 +2037,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E38" s="11" t="n">
         <v>4</v>
@@ -2036,10 +2071,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E39" s="11" t="n">
         <v>3</v>
@@ -2070,16 +2105,20 @@
         <v>1</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E40" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="10"/>
+      <c r="F40" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="H40" s="10" t="n">
         <v>1</v>
       </c>
@@ -2108,10 +2147,10 @@
         <v>3</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E41" s="11" t="n">
         <v>4</v>
@@ -2188,7 +2227,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="11" t="n">
         <f aca="false">E7*H7+E8*H8+E9*H9+E10*H10+E11*H11+E12*H12+E13*H13+E14*H14+E15*H15+E16*H16+E17*H17+E18*H18+E19*H19+E20*H20+E21*H21+E22*H22+E25*H25+E26*H26+E27*H27+E30*H30+E31*H31+E32*H32+E33*H33+E36*H36+E37*H37+E38*H38+E39*H39+E40*H40+E41*H41</f>
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2213,7 +2252,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="22"/>
       <c r="D45" s="23" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E45" s="11" t="n">
         <f aca="false">SUM(E7:E22)+SUM(E25:E27)+SUM(E30:E33)+SUM(E36:E41)</f>

</xml_diff>

<commit_message>
csrf + fix + doc
</commit_message>
<xml_diff>
--- a/conception/LBS-stories-LP1.xlsx
+++ b/conception/LBS-stories-LP1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -285,6 +285,12 @@
     <t xml:space="preserve">créer une carte de fidélité – retourne un identifiant de carte </t>
   </si>
   <si>
+    <t xml:space="preserve">/carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel /Baptiste/Islam</t>
+  </si>
+  <si>
     <t xml:space="preserve">STORIES CONCERNANT LE BACKEND DE GESTION</t>
   </si>
   <si>
@@ -307,6 +313,9 @@
   </si>
   <si>
     <t xml:space="preserve">ajouter un sandwich dans la liste, en indiquant sa catégorie – gérer le token csrf – gérer les tailles et prix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/add_sandwich</t>
   </si>
   <si>
     <t xml:space="preserve">modifier 1 sandwich</t>
@@ -630,8 +639,8 @@
   </sheetPr>
   <dimension ref="A1:V65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,7 +653,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.765306122449"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.0612244897959"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.9132653061224"/>
     <col collapsed="false" hidden="false" max="22" min="10" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.23469387755102"/>
   </cols>
@@ -1871,10 +1880,18 @@
       <c r="E33" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
+      <c r="F33" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -1891,7 +1908,7 @@
     </row>
     <row r="34" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -1961,10 +1978,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E36" s="11" t="n">
         <v>3</v>
@@ -1973,7 +1990,7 @@
         <v>13</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H36" s="10" t="n">
         <v>1</v>
@@ -2003,10 +2020,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E37" s="11" t="n">
         <v>4</v>
@@ -2037,18 +2054,26 @@
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E38" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
+      <c r="F38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H38" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -2071,10 +2096,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E39" s="11" t="n">
         <v>3</v>
@@ -2105,10 +2130,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E40" s="11" t="n">
         <v>4</v>
@@ -2117,7 +2142,7 @@
         <v>38</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H40" s="10" t="n">
         <v>1</v>
@@ -2147,10 +2172,10 @@
         <v>3</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E41" s="11" t="n">
         <v>4</v>
@@ -2227,7 +2252,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="11" t="n">
         <f aca="false">E7*H7+E8*H8+E9*H9+E10*H10+E11*H11+E12*H12+E13*H13+E14*H14+E15*H15+E16*H16+E17*H17+E18*H18+E19*H19+E20*H20+E21*H21+E22*H22+E25*H25+E26*H26+E27*H27+E30*H30+E31*H31+E32*H32+E33*H33+E36*H36+E37*H37+E38*H38+E39*H39+E40*H40+E41*H41</f>
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2252,7 +2277,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="22"/>
       <c r="D45" s="23" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E45" s="11" t="n">
         <f aca="false">SUM(E7:E22)+SUM(E25:E27)+SUM(E30:E33)+SUM(E36:E41)</f>

</xml_diff>